<commit_message>
added some function in DomiDisplay
</commit_message>
<xml_diff>
--- a/DomiDisplay/database/docTemplate.xlsx
+++ b/DomiDisplay/database/docTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="14000"/>
+    <workbookView windowWidth="28000" windowHeight="13260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -198,10 +198,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -214,13 +214,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,6 +234,84 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -249,65 +320,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -320,37 +343,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -365,187 +365,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,24 +568,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -597,6 +579,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -642,17 +648,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -661,145 +661,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1131,8 +1131,8 @@
   <sheetPr/>
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="13.6" outlineLevelCol="1"/>
@@ -1150,7 +1150,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1158,7 +1158,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1166,7 +1166,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1174,7 +1174,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1182,7 +1182,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1190,7 +1190,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1198,7 +1198,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1206,7 +1206,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1214,7 +1214,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1222,7 +1222,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1230,7 +1230,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1238,7 +1238,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1246,7 +1246,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>13</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1254,7 +1254,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1262,7 +1262,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1270,7 +1270,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>16</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1278,7 +1278,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>17</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1286,7 +1286,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>18</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1294,7 +1294,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>19</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1302,7 +1302,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1310,7 +1310,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>21</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1318,7 +1318,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>22</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1326,7 +1326,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>23</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1334,7 +1334,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>24</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1342,7 +1342,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>25</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1350,7 +1350,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>26</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1358,7 +1358,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>27</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1366,7 +1366,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>28</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1374,7 +1374,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>29</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1382,7 +1382,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>30</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1390,7 +1390,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>31</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1398,7 +1398,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>32</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1406,7 +1406,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>33</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1414,7 +1414,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>34</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1422,7 +1422,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>35</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1430,7 +1430,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>36</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1438,7 +1438,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>37</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1446,7 +1446,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>38</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1454,7 +1454,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>39</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1462,7 +1462,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>40</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1470,7 +1470,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>41</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1478,7 +1478,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>42</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1486,7 +1486,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>43</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1494,7 +1494,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>44</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1502,7 +1502,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>45</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1510,7 +1510,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>46</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1518,7 +1518,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>47</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1526,7 +1526,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>48</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1534,7 +1534,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>49</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1542,7 +1542,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>50</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1550,7 +1550,7 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>51</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1558,7 +1558,7 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>52</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1566,7 +1566,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>53</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1574,7 +1574,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>54</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1582,7 +1582,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>55</v>
+        <v>154</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1590,7 +1590,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>56</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1598,7 +1598,7 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>57</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>